<commit_message>
find bug for upgrade house will cause citizen not right
</commit_message>
<xml_diff>
--- a/gameData/server/PlayerInitData.xlsx
+++ b/gameData/server/PlayerInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="980" windowWidth="28540" windowHeight="19080" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="6500" yWindow="5020" windowWidth="19640" windowHeight="14540" tabRatio="883" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="resources" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -57,23 +57,38 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>INT_tools</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_tiles</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_pulley</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_level</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>INT_blueprints</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_tools</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_tiles</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_pulley</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_level</t>
+    <t>INT_trainingFigure</t>
+  </si>
+  <si>
+    <t>INT_bowTarget</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_saddle</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_ironPart</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -748,7 +763,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -818,10 +833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -829,24 +844,36 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" spans="1:9" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -860,6 +887,18 @@
         <v>1000</v>
       </c>
       <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="1">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move gem from basicInfo to resoruces add cart to resources
</commit_message>
<xml_diff>
--- a/gameData/server/PlayerInitData.xlsx
+++ b/gameData/server/PlayerInitData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="5020" windowWidth="19640" windowHeight="14540" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="8140" yWindow="23180" windowWidth="19640" windowHeight="14540" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="resources" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -89,6 +89,10 @@
   </si>
   <si>
     <t>INT_ironPart</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_cart</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -750,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -761,7 +765,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -786,8 +790,11 @@
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="20" customHeight="1">
+    <row r="2" spans="1:9" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -812,11 +819,14 @@
       <c r="H2" s="1">
         <v>50000</v>
       </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="20" customHeight="1">
+    <row r="3" spans="1:9" ht="20" customHeight="1">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="20" customHeight="1">
+    <row r="4" spans="1:9" ht="20" customHeight="1">
       <c r="B4" s="2"/>
     </row>
   </sheetData>
@@ -835,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>